<commit_message>
Schematic revision for DAC board, compensation tweaks in lv_regs.
Opamp +/- pins were swapped in reference_buffer.sch as side effect of the symbol change from using a dual opamp.

lv_regs files.  The compensation components were (CTUNE/RTUNE) were quite wrong, and everything oscillated like crazy. The positive regulators are fine with no compensation, and the negative regulator benefits from a bit.
</commit_message>
<xml_diff>
--- a/docs/timeline.xlsx
+++ b/docs/timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_hw\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7FC60C-B6FC-4F82-B078-6AAD3E4EBBBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC97ABE-8652-4275-BA6D-0C5587A675E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="0" windowWidth="16230" windowHeight="12960" xr2:uid="{9027C169-0E65-48AF-A2B2-577F81CFB246}"/>
+    <workbookView xWindow="8940" yWindow="3735" windowWidth="19980" windowHeight="11835" xr2:uid="{9027C169-0E65-48AF-A2B2-577F81CFB246}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -144,10 +144,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,18 +466,18 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="57.28515625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="5" max="5" width="35.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -504,11 +504,11 @@
       <c r="D2" s="1">
         <v>43987</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -518,9 +518,9 @@
       <c r="D3" s="1">
         <v>44008</v>
       </c>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -530,9 +530,9 @@
       <c r="D4" s="1">
         <v>44011</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -542,9 +542,9 @@
       <c r="D5" s="1">
         <v>44025</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -554,9 +554,9 @@
       <c r="D6" s="1">
         <v>44046</v>
       </c>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -569,11 +569,11 @@
       <c r="D9" s="1">
         <v>44027</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>12</v>
       </c>
@@ -583,9 +583,9 @@
       <c r="D10" s="1">
         <v>44048</v>
       </c>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -595,9 +595,9 @@
       <c r="D11" s="1">
         <v>44105</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -607,9 +607,9 @@
       <c r="D12" s="1">
         <v>44150</v>
       </c>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -619,9 +619,9 @@
       <c r="D13" s="1">
         <v>44166</v>
       </c>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>18</v>
       </c>
@@ -631,9 +631,9 @@
       <c r="D14" s="1">
         <v>43876</v>
       </c>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -647,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>22</v>
       </c>

</xml_diff>